<commit_message>
Additional data for #97
</commit_message>
<xml_diff>
--- a/Documents/Plancrow-Calculations.xlsx
+++ b/Documents/Plancrow-Calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
   <si>
     <t>Y1</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>NPV</t>
-  </si>
-  <si>
-    <t>Size 5-10</t>
   </si>
   <si>
     <t>Tax @ 30%</t>
@@ -580,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,21 +590,21 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -651,7 +648,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -666,7 +663,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
@@ -681,7 +678,7 @@
         <v>400</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
@@ -805,7 +802,7 @@
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -820,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -835,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N8" s="3">
         <v>0</v>
@@ -896,7 +893,7 @@
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -912,7 +909,7 @@
         <v>2880</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3">
@@ -928,7 +925,7 @@
         <v>19200</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3">
@@ -946,7 +943,7 @@
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -959,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -968,7 +965,7 @@
         <v>10000</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3">
@@ -983,7 +980,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -996,7 +993,7 @@
         <v>2000</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
@@ -1009,7 +1006,7 @@
         <v>4000</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3">
@@ -1160,7 +1157,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -1176,7 +1173,7 @@
         <v>1304</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
@@ -1192,7 +1189,7 @@
         <v>2960</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3">
@@ -1531,7 +1528,7 @@
     </row>
     <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="12">
@@ -1548,7 +1545,7 @@
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="12">
@@ -1565,7 +1562,7 @@
       </c>
       <c r="L26" s="11"/>
       <c r="M26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N26" s="11"/>
       <c r="O26" s="12">

</xml_diff>